<commit_message>
[MOD] Tracion coeffifcient formulation changed
</commit_message>
<xml_diff>
--- a/parameters/BAJA.xlsx
+++ b/parameters/BAJA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulo\Desktop\TIA\parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D534F841-2FBF-4C78-9EC0-7027C5A5B01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69344E7C-07E9-4FA3-98C5-CAE76DD60D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Front</t>
   </si>
@@ -51,18 +51,12 @@
     <t>none</t>
   </si>
   <si>
-    <t>Pedal - Cylinder ratio</t>
-  </si>
-  <si>
     <t>Amc</t>
   </si>
   <si>
     <t>cm²</t>
   </si>
   <si>
-    <t>Marter cylider cross section area</t>
-  </si>
-  <si>
     <t>Awc</t>
   </si>
   <si>
@@ -81,9 +75,6 @@
     <t>Hp</t>
   </si>
   <si>
-    <t>Brake bobings height</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -103,6 +94,9 @@
   </si>
   <si>
     <t>15.8</t>
+  </si>
+  <si>
+    <t>Brake pad height</t>
   </si>
 </sst>
 </file>
@@ -240,7 +234,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="3" applyFont="1"/>
@@ -264,9 +258,6 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
@@ -553,19 +544,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="12" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="10" t="s">
         <v>0</v>
@@ -577,7 +569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -592,58 +584,58 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="B5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="B6" s="11">
         <v>95</v>
@@ -652,15 +644,15 @@
         <v>95</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="B7" s="11">
         <v>40</v>
@@ -669,15 +661,15 @@
         <v>40</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B8" s="11">
         <v>224</v>
@@ -686,73 +678,46 @@
         <v>224</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>18</v>
-      </c>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>20</v>
-      </c>
+      <c r="A17" s="9"/>
+      <c r="B17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G18" s="6"/>

</xml_diff>